<commit_message>
started new version of prioritization doc
</commit_message>
<xml_diff>
--- a/data/derived_data/Master Sites Table_07262022.xlsx
+++ b/data/derived_data/Master Sites Table_07262022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\SnakeR_IPTDS\data\derived_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C113B61-4FF7-4AFE-B3A8-BCA5CC618D24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39376CB3-F828-4C97-ADAD-EA7C3E378C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="54600" yWindow="-2385" windowWidth="25800" windowHeight="21150" tabRatio="753" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="16440" windowHeight="28590" tabRatio="753" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Integrated O&amp;M Sites" sheetId="1" r:id="rId1"/>
@@ -2264,7 +2264,19 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2283,18 +2295,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2670,10 +2670,10 @@
   <dimension ref="A1:AY61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B22" activeCellId="1" sqref="B35:B48 B3:B22"/>
+      <selection pane="bottomRight" activeCell="AX50" sqref="AX50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="13" x14ac:dyDescent="0.3"/>
@@ -2733,66 +2733,66 @@
     <row r="1" spans="1:51" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30"/>
       <c r="B1" s="30"/>
-      <c r="C1" s="67" t="s">
+      <c r="C1" s="68" t="s">
         <v>251</v>
       </c>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67" t="s">
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68" t="s">
         <v>250</v>
       </c>
-      <c r="G1" s="67"/>
-      <c r="H1" s="67"/>
-      <c r="I1" s="67"/>
-      <c r="J1" s="75" t="s">
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="69" t="s">
         <v>248</v>
       </c>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="71" t="s">
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="75" t="s">
         <v>249</v>
       </c>
-      <c r="V1" s="72"/>
-      <c r="W1" s="72"/>
-      <c r="X1" s="72"/>
-      <c r="Y1" s="72"/>
-      <c r="Z1" s="72"/>
-      <c r="AA1" s="72"/>
-      <c r="AB1" s="72"/>
-      <c r="AC1" s="72"/>
-      <c r="AD1" s="73"/>
-      <c r="AE1" s="67" t="s">
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="76"/>
+      <c r="AA1" s="76"/>
+      <c r="AB1" s="76"/>
+      <c r="AC1" s="76"/>
+      <c r="AD1" s="77"/>
+      <c r="AE1" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="AF1" s="67"/>
-      <c r="AG1" s="67"/>
+      <c r="AF1" s="68"/>
+      <c r="AG1" s="68"/>
       <c r="AH1" s="21"/>
-      <c r="AI1" s="67" t="s">
+      <c r="AI1" s="68" t="s">
         <v>233</v>
       </c>
-      <c r="AJ1" s="67"/>
-      <c r="AK1" s="67"/>
-      <c r="AL1" s="67"/>
-      <c r="AM1" s="67"/>
-      <c r="AN1" s="67"/>
-      <c r="AO1" s="67"/>
-      <c r="AP1" s="67"/>
+      <c r="AJ1" s="68"/>
+      <c r="AK1" s="68"/>
+      <c r="AL1" s="68"/>
+      <c r="AM1" s="68"/>
+      <c r="AN1" s="68"/>
+      <c r="AO1" s="68"/>
+      <c r="AP1" s="68"/>
       <c r="AQ1" s="21"/>
-      <c r="AR1" s="68" t="s">
+      <c r="AR1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="AS1" s="69"/>
-      <c r="AT1" s="69"/>
-      <c r="AU1" s="69"/>
-      <c r="AV1" s="70"/>
+      <c r="AS1" s="73"/>
+      <c r="AT1" s="73"/>
+      <c r="AU1" s="73"/>
+      <c r="AV1" s="74"/>
       <c r="AW1" s="54"/>
       <c r="AX1" s="26" t="s">
         <v>1</v>
@@ -10162,7 +10162,7 @@
         <f>COUNTA(S3:S46)</f>
         <v>18</v>
       </c>
-      <c r="V50" s="74" t="s">
+      <c r="V50" s="67" t="s">
         <v>517</v>
       </c>
       <c r="W50" s="6" t="s">
@@ -10264,7 +10264,7 @@
       <c r="S51" s="48" t="s">
         <v>485</v>
       </c>
-      <c r="V51" s="74"/>
+      <c r="V51" s="67"/>
       <c r="W51" s="6" t="s">
         <v>516</v>
       </c>
@@ -10291,7 +10291,7 @@
         <f>COUNTIF(J3:J48, "5060 Hybrid TEG")</f>
         <v>5</v>
       </c>
-      <c r="V52" s="74"/>
+      <c r="V52" s="67"/>
       <c r="W52" s="6" t="s">
         <v>93</v>
       </c>
@@ -10316,7 +10316,7 @@
         <f>COUNTIF(J3:J48, "Grid Power")+ COUNTIF(J3:J48, "Grid Power - Cust.")+ COUNTIF(J3:J48, "Grid Power PLC")</f>
         <v>23</v>
       </c>
-      <c r="V53" s="74"/>
+      <c r="V53" s="67"/>
       <c r="W53" s="6" t="s">
         <v>111</v>
       </c>
@@ -10345,7 +10345,7 @@
     </row>
     <row r="55" spans="1:51" x14ac:dyDescent="0.3">
       <c r="B55" s="6"/>
-      <c r="V55" s="74" t="s">
+      <c r="V55" s="67" t="s">
         <v>518</v>
       </c>
       <c r="W55" s="6" t="s">
@@ -10358,7 +10358,7 @@
     </row>
     <row r="56" spans="1:51" x14ac:dyDescent="0.3">
       <c r="B56" s="6"/>
-      <c r="V56" s="74"/>
+      <c r="V56" s="67"/>
       <c r="W56" s="6" t="s">
         <v>516</v>
       </c>
@@ -10368,7 +10368,7 @@
       </c>
     </row>
     <row r="58" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="V58" s="74" t="s">
+      <c r="V58" s="67" t="s">
         <v>9</v>
       </c>
       <c r="W58" s="6" t="s">
@@ -10380,7 +10380,7 @@
       </c>
     </row>
     <row r="59" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="V59" s="74"/>
+      <c r="V59" s="67"/>
       <c r="W59" s="6" t="s">
         <v>516</v>
       </c>
@@ -10390,7 +10390,7 @@
       </c>
     </row>
     <row r="60" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="V60" s="74"/>
+      <c r="V60" s="67"/>
       <c r="W60" s="6" t="s">
         <v>93</v>
       </c>
@@ -10399,7 +10399,7 @@
       </c>
     </row>
     <row r="61" spans="1:51" x14ac:dyDescent="0.3">
-      <c r="V61" s="74"/>
+      <c r="V61" s="67"/>
       <c r="W61" s="6" t="s">
         <v>111</v>
       </c>
@@ -10408,23 +10408,22 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AY2" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:AX44">
     <sortCondition ref="D3:D44"/>
     <sortCondition ref="E3:E44"/>
     <sortCondition ref="B3:B44"/>
   </sortState>
   <mergeCells count="10">
+    <mergeCell ref="AI1:AP1"/>
+    <mergeCell ref="AR1:AV1"/>
+    <mergeCell ref="AE1:AG1"/>
+    <mergeCell ref="U1:AD1"/>
+    <mergeCell ref="F1:I1"/>
     <mergeCell ref="V50:V53"/>
     <mergeCell ref="V55:V56"/>
     <mergeCell ref="V58:V61"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="J1:T1"/>
-    <mergeCell ref="AI1:AP1"/>
-    <mergeCell ref="AR1:AV1"/>
-    <mergeCell ref="AE1:AG1"/>
-    <mergeCell ref="U1:AD1"/>
-    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
@@ -10442,7 +10441,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AW50"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="AP53" sqref="AP53"/>
     </sheetView>
   </sheetViews>
@@ -12148,31 +12147,31 @@
       <c r="G1" s="78"/>
       <c r="H1" s="78"/>
       <c r="I1" s="78"/>
-      <c r="J1" s="75" t="s">
+      <c r="J1" s="69" t="s">
         <v>248</v>
       </c>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-      <c r="S1" s="76"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="75" t="s">
+      <c r="K1" s="70"/>
+      <c r="L1" s="70"/>
+      <c r="M1" s="70"/>
+      <c r="N1" s="70"/>
+      <c r="O1" s="70"/>
+      <c r="P1" s="70"/>
+      <c r="Q1" s="70"/>
+      <c r="R1" s="70"/>
+      <c r="S1" s="70"/>
+      <c r="T1" s="71"/>
+      <c r="U1" s="69" t="s">
         <v>249</v>
       </c>
-      <c r="V1" s="76"/>
-      <c r="W1" s="76"/>
-      <c r="X1" s="76"/>
-      <c r="Y1" s="76"/>
-      <c r="Z1" s="76"/>
-      <c r="AA1" s="76"/>
-      <c r="AB1" s="76"/>
-      <c r="AC1" s="76"/>
-      <c r="AD1" s="77"/>
+      <c r="V1" s="70"/>
+      <c r="W1" s="70"/>
+      <c r="X1" s="70"/>
+      <c r="Y1" s="70"/>
+      <c r="Z1" s="70"/>
+      <c r="AA1" s="70"/>
+      <c r="AB1" s="70"/>
+      <c r="AC1" s="70"/>
+      <c r="AD1" s="71"/>
       <c r="AE1" s="78" t="s">
         <v>8</v>
       </c>
@@ -22759,12 +22758,9 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<sisl xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="http://www.boldonjames.com/2008/01/sie/internal/label" sislVersion="0" policy="a10f9ac0-5937-4b4f-b459-96aedd9ed2c5" origin="userSelected">
+  <element uid="9920fcc9-9f43-4d43-9e3e-b98a219cfd55" value=""/>
+</sisl>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22787,9 +22783,12 @@
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<sisl xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="http://www.boldonjames.com/2008/01/sie/internal/label" sislVersion="0" policy="a10f9ac0-5937-4b4f-b459-96aedd9ed2c5" origin="userSelected">
-  <element uid="9920fcc9-9f43-4d43-9e3e-b98a219cfd55" value=""/>
-</sisl>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22812,9 +22811,10 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4688D02-0DEF-4234-9A74-2AE1D20FF3AE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{894378A2-7747-4470-AA17-0EF4D0A08B98}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -22837,10 +22837,9 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{894378A2-7747-4470-AA17-0EF4D0A08B98}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E4688D02-0DEF-4234-9A74-2AE1D20FF3AE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://www.boldonjames.com/2008/01/sie/internal/label"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>